<commit_message>
Mettre à à jour l'inventaire
Par l'introduction de 13 clés USB
</commit_message>
<xml_diff>
--- a/divers/Inventaire.xlsx
+++ b/divers/Inventaire.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,50 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Clé USB 1</t>
+  </si>
+  <si>
+    <t>Clé USB 2</t>
+  </si>
+  <si>
+    <t>Clé USB 3</t>
+  </si>
+  <si>
+    <t>Clé USB 4</t>
+  </si>
+  <si>
+    <t>Clé USB 5</t>
+  </si>
+  <si>
+    <t>Clé USB 6</t>
+  </si>
+  <si>
+    <t>Clé USB 7</t>
+  </si>
+  <si>
+    <t>Clé USB 8</t>
+  </si>
+  <si>
+    <t>Clé USB 9</t>
+  </si>
+  <si>
+    <t>Clé USB 10</t>
+  </si>
+  <si>
+    <t>Clé USB 11</t>
+  </si>
+  <si>
+    <t>Clé USB 12</t>
+  </si>
+  <si>
+    <t>Clé USB 13</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -69,7 +113,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +158,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +193,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,12 +375,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>